<commit_message>
updated log of testing
</commit_message>
<xml_diff>
--- a/Docs/log_debug.xlsx
+++ b/Docs/log_debug.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="21">
   <si>
     <t>k</t>
   </si>
@@ -96,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +114,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -231,6 +238,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2497,16 +2506,18 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2652,7 +2663,7 @@
       <c r="F7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="18">
         <v>0.19400000000000001</v>
       </c>
     </row>
@@ -2711,8 +2722,12 @@
       <c r="E10" s="11">
         <v>0</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="13"/>
+      <c r="F10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4">
+        <v>-0.14799999999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -2726,34 +2741,50 @@
       <c r="E11" s="7">
         <v>1</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="4"/>
+      <c r="F11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="4">
+        <v>-0.39400000000000002</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
       <c r="D12" s="7">
         <v>0</v>
       </c>
       <c r="E12" s="7">
         <v>0</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="13">
+        <v>3.093</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
       <c r="D13" s="7">
         <v>0</v>
       </c>
       <c r="E13" s="7">
         <v>1</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="2"/>
+      <c r="F13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -2772,7 +2803,9 @@
       <c r="F14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="2"/>
+      <c r="G14" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -2808,7 +2841,9 @@
       <c r="F16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="17">
+        <v>2.71</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -2843,8 +2878,12 @@
       <c r="E18" s="7">
         <v>0</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="4"/>
+      <c r="F18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1.038</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -2858,8 +2897,12 @@
       <c r="E19" s="7">
         <v>1</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="4"/>
+      <c r="F19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="4">
+        <v>-0.2</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -2873,8 +2916,12 @@
       <c r="E20" s="7">
         <v>0</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="4"/>
+      <c r="F20" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1.5349999999999999</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -2888,36 +2935,88 @@
       <c r="E21" s="7">
         <v>1</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="4"/>
+      <c r="F21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0.89400000000000002</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7">
+        <v>20</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="4">
+        <v>-0.73699999999999999</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7">
+        <v>20</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="4">
+        <v>-0.21</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7">
+        <v>0</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="4">
+        <v>-0.26</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="4">
+        <v>9.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>

</xml_diff>